<commit_message>
FINAL CLEAN-UP! READY TO LAUNCH
</commit_message>
<xml_diff>
--- a/cansat-arduino/cansat-rx/finaldata.xlsx
+++ b/cansat-arduino/cansat-rx/finaldata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,34 +492,34 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>24</v>
+        <v>30.803</v>
       </c>
       <c r="B2" t="n">
-        <v>24367</v>
+        <v>30803</v>
       </c>
       <c r="C2" t="n">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D2" t="n">
-        <v>17.68</v>
+        <v>18.38</v>
       </c>
       <c r="E2" t="n">
-        <v>954.4400000000001</v>
+        <v>960.62</v>
       </c>
       <c r="F2" t="n">
-        <v>558.09</v>
+        <v>548.79</v>
       </c>
       <c r="G2" t="n">
-        <v>0.04</v>
+        <v>2.98</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.2</v>
+        <v>0.67</v>
       </c>
       <c r="I2" t="n">
-        <v>11.38</v>
+        <v>-8.390000000000001</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>5.851108989930826</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -527,1647 +527,1542 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>26</v>
+        <v>32.412</v>
       </c>
       <c r="B3" t="n">
-        <v>25976</v>
+        <v>32412</v>
       </c>
       <c r="C3" t="n">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="D3" t="n">
-        <v>17.69</v>
+        <v>18.4</v>
       </c>
       <c r="E3" t="n">
-        <v>954.45</v>
+        <v>960.61</v>
       </c>
       <c r="F3" t="n">
-        <v>558.05</v>
+        <v>548.8099999999999</v>
       </c>
       <c r="G3" t="n">
-        <v>0.08</v>
+        <v>3.45</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.24</v>
+        <v>0.82</v>
       </c>
       <c r="I3" t="n">
-        <v>11.41</v>
+        <v>-7.85</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>5.067425419723871</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.0200000000000386</v>
+        <v>0.0124300807955138</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>28</v>
+        <v>34.021</v>
       </c>
       <c r="B4" t="n">
-        <v>27585</v>
+        <v>34021</v>
       </c>
       <c r="C4" t="n">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="D4" t="n">
-        <v>17.69</v>
+        <v>18.43</v>
       </c>
       <c r="E4" t="n">
-        <v>954.45</v>
+        <v>960.61</v>
       </c>
       <c r="F4" t="n">
-        <v>558.0700000000001</v>
+        <v>548.84</v>
       </c>
       <c r="G4" t="n">
-        <v>0.04</v>
+        <v>2.28</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.16</v>
+        <v>0.75</v>
       </c>
       <c r="I4" t="n">
-        <v>11.34</v>
+        <v>-6.86</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>4.137768110863971</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0100000000000477</v>
+        <v>0.0186451211933414</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>29</v>
+        <v>35.631</v>
       </c>
       <c r="B5" t="n">
-        <v>29194</v>
+        <v>35631</v>
       </c>
       <c r="C5" t="n">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="D5" t="n">
-        <v>17.7</v>
+        <v>18.45</v>
       </c>
       <c r="E5" t="n">
-        <v>954.45</v>
+        <v>960.6</v>
       </c>
       <c r="F5" t="n">
-        <v>558.04</v>
+        <v>548.9299999999999</v>
       </c>
       <c r="G5" t="n">
-        <v>0.04</v>
+        <v>2.12</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.24</v>
+        <v>-0.08</v>
       </c>
       <c r="I5" t="n">
-        <v>11.41</v>
+        <v>-8.119999999999999</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>5.067926703787494</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.0300000000000864</v>
+        <v>0.0559006211179616</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>31</v>
+        <v>37.24</v>
       </c>
       <c r="B6" t="n">
-        <v>30803</v>
+        <v>37240</v>
       </c>
       <c r="C6" t="n">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D6" t="n">
-        <v>17.71</v>
+        <v>18.47</v>
       </c>
       <c r="E6" t="n">
-        <v>954.45</v>
+        <v>960.59</v>
       </c>
       <c r="F6" t="n">
-        <v>558.04</v>
+        <v>549</v>
       </c>
       <c r="G6" t="n">
-        <v>0.04</v>
+        <v>1.92</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.27</v>
+        <v>-1.41</v>
       </c>
       <c r="I6" t="n">
-        <v>11.41</v>
+        <v>-8.470000000000001</v>
       </c>
       <c r="J6" t="n">
-        <v>2.936041142894189</v>
+        <v>5.068143150515303</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>0.0435052827843691</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>32</v>
+        <v>40.458</v>
       </c>
       <c r="B7" t="n">
-        <v>32412</v>
+        <v>40458</v>
       </c>
       <c r="C7" t="n">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D7" t="n">
-        <v>17.71</v>
+        <v>18.51</v>
       </c>
       <c r="E7" t="n">
-        <v>954.46</v>
+        <v>960.5700000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>557.98</v>
+        <v>549.16</v>
       </c>
       <c r="G7" t="n">
-        <v>0.04</v>
+        <v>3.06</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.2</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="I7" t="n">
-        <v>11.38</v>
+        <v>-8.24</v>
       </c>
       <c r="J7" t="n">
-        <v>2.936025637780515</v>
+        <v>5.068576091237688</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.0599999999999454</v>
+        <v>0.0497203231820908</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>34</v>
+        <v>42.067</v>
       </c>
       <c r="B8" t="n">
-        <v>34021</v>
+        <v>42067</v>
       </c>
       <c r="C8" t="n">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="D8" t="n">
-        <v>17.72</v>
+        <v>18.53</v>
       </c>
       <c r="E8" t="n">
-        <v>954.46</v>
+        <v>960.59</v>
       </c>
       <c r="F8" t="n">
-        <v>557.95</v>
+        <v>548.98</v>
       </c>
       <c r="G8" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="H8" t="n">
         <v>0.08</v>
       </c>
-      <c r="H8" t="n">
-        <v>-0.24</v>
-      </c>
       <c r="I8" t="n">
-        <v>11.38</v>
+        <v>-6.63</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>5.06871302932237</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0149999999999863</v>
+        <v>-0.1118707271596953</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>36</v>
+        <v>43.676</v>
       </c>
       <c r="B9" t="n">
-        <v>35630</v>
+        <v>43676</v>
       </c>
       <c r="C9" t="n">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D9" t="n">
-        <v>17.73</v>
+        <v>18.55</v>
       </c>
       <c r="E9" t="n">
-        <v>954.46</v>
+        <v>960.62</v>
       </c>
       <c r="F9" t="n">
-        <v>557.95</v>
+        <v>548.77</v>
       </c>
       <c r="G9" t="n">
-        <v>0.04</v>
+        <v>2.43</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.2</v>
+        <v>-0.9399999999999999</v>
       </c>
       <c r="I9" t="n">
-        <v>11.38</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>5.852973177443198</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>-0.1305158483530367</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>37</v>
+        <v>45.285</v>
       </c>
       <c r="B10" t="n">
-        <v>37239</v>
+        <v>45285</v>
       </c>
       <c r="C10" t="n">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D10" t="n">
-        <v>17.73</v>
+        <v>18.59</v>
       </c>
       <c r="E10" t="n">
-        <v>954.46</v>
+        <v>960.65</v>
       </c>
       <c r="F10" t="n">
-        <v>557.9299999999999</v>
+        <v>548.5</v>
       </c>
       <c r="G10" t="n">
-        <v>0.04</v>
+        <v>2.39</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.24</v>
+        <v>-1.29</v>
       </c>
       <c r="I10" t="n">
-        <v>11.34</v>
+        <v>-9.26</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>5.853320101184092</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0200000000000954</v>
+        <v>-0.167806090739579</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>39</v>
+        <v>50.112</v>
       </c>
       <c r="B11" t="n">
-        <v>38849</v>
+        <v>50112</v>
       </c>
       <c r="C11" t="n">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="D11" t="n">
-        <v>17.74</v>
+        <v>18.68</v>
       </c>
       <c r="E11" t="n">
-        <v>954.46</v>
+        <v>960.66</v>
       </c>
       <c r="F11" t="n">
-        <v>557.9299999999999</v>
+        <v>548.41</v>
       </c>
       <c r="G11" t="n">
-        <v>0.04</v>
+        <v>1.88</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.16</v>
+        <v>-0.9</v>
       </c>
       <c r="I11" t="n">
-        <v>11.38</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="J11" t="n">
-        <v>2.936199521102561</v>
+        <v>5.069952564828553</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>-0.0186451211932943</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>40</v>
+        <v>58.157</v>
       </c>
       <c r="B12" t="n">
-        <v>40458</v>
+        <v>58157</v>
       </c>
       <c r="C12" t="n">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="D12" t="n">
-        <v>17.74</v>
+        <v>18.87</v>
       </c>
       <c r="E12" t="n">
-        <v>954.47</v>
+        <v>960.66</v>
       </c>
       <c r="F12" t="n">
-        <v>557.89</v>
+        <v>548.41</v>
       </c>
       <c r="G12" t="n">
-        <v>0.04</v>
+        <v>1.88</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.16</v>
+        <v>-1.22</v>
       </c>
       <c r="I12" t="n">
-        <v>11.38</v>
+        <v>-5.26</v>
       </c>
       <c r="J12" t="n">
+        <v>4.141073739450332</v>
+      </c>
+      <c r="K12" t="n">
         <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>-0.0399999999999636</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>42</v>
+        <v>59.766</v>
       </c>
       <c r="B13" t="n">
-        <v>42067</v>
+        <v>59766</v>
       </c>
       <c r="C13" t="n">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="D13" t="n">
-        <v>17.75</v>
+        <v>18.92</v>
       </c>
       <c r="E13" t="n">
-        <v>954.47</v>
+        <v>960.66</v>
       </c>
       <c r="F13" t="n">
-        <v>557.9</v>
+        <v>548.42</v>
       </c>
       <c r="G13" t="n">
-        <v>0.04</v>
+        <v>2.08</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.16</v>
+        <v>-2.86</v>
       </c>
       <c r="I13" t="n">
-        <v>11.34</v>
+        <v>-9.57</v>
       </c>
       <c r="J13" t="n">
-        <v>2.936241982964264</v>
+        <v>5.856911741857761</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0049999999999954</v>
+        <v>0.0062150403977569</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>44</v>
+        <v>61.375</v>
       </c>
       <c r="B14" t="n">
-        <v>43676</v>
+        <v>61375</v>
       </c>
       <c r="C14" t="n">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="D14" t="n">
-        <v>17.75</v>
+        <v>18.96</v>
       </c>
       <c r="E14" t="n">
-        <v>954.46</v>
+        <v>960.65</v>
       </c>
       <c r="F14" t="n">
-        <v>557.92</v>
+        <v>548.49</v>
       </c>
       <c r="G14" t="n">
-        <v>0.08</v>
+        <v>2.39</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.24</v>
+        <v>-5.06</v>
       </c>
       <c r="I14" t="n">
-        <v>11.38</v>
+        <v>-5.3</v>
       </c>
       <c r="J14" t="n">
-        <v>2.936257489373248</v>
+        <v>5.072641382434636</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0099999999999909</v>
+        <v>0.0435052827843691</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>45</v>
+        <v>62.984</v>
       </c>
       <c r="B15" t="n">
-        <v>45285</v>
+        <v>62984</v>
       </c>
       <c r="C15" t="n">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="D15" t="n">
-        <v>17.76</v>
+        <v>19</v>
       </c>
       <c r="E15" t="n">
-        <v>954.46</v>
+        <v>960.66</v>
       </c>
       <c r="F15" t="n">
-        <v>557.95</v>
+        <v>548.4400000000001</v>
       </c>
       <c r="G15" t="n">
-        <v>-2.43</v>
+        <v>0.71</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.31</v>
+        <v>0.51</v>
       </c>
       <c r="I15" t="n">
-        <v>10.36</v>
+        <v>-8.279999999999999</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>5.072995381844846</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0300000000000864</v>
+        <v>-0.0310752019887846</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>49</v>
+        <v>64.593</v>
       </c>
       <c r="B16" t="n">
-        <v>48503</v>
+        <v>64593</v>
       </c>
       <c r="C16" t="n">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="D16" t="n">
-        <v>17.77</v>
+        <v>19.04</v>
       </c>
       <c r="E16" t="n">
-        <v>954.45</v>
+        <v>960.66</v>
       </c>
       <c r="F16" t="n">
-        <v>558.03</v>
+        <v>548.4299999999999</v>
       </c>
       <c r="G16" t="n">
-        <v>-1.22</v>
+        <v>1.26</v>
       </c>
       <c r="H16" t="n">
-        <v>-1.22</v>
+        <v>0.27</v>
       </c>
       <c r="I16" t="n">
-        <v>10.36</v>
+        <v>-8.83</v>
       </c>
       <c r="J16" t="n">
-        <v>2.936388944098884</v>
+        <v>5.858229970592848</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0199999999999818</v>
+        <v>-0.0062150403978275</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>50</v>
+        <v>66.202</v>
       </c>
       <c r="B17" t="n">
-        <v>50112</v>
+        <v>66202</v>
       </c>
       <c r="C17" t="n">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="D17" t="n">
-        <v>17.77</v>
+        <v>19.07</v>
       </c>
       <c r="E17" t="n">
-        <v>954.4400000000001</v>
+        <v>960.66</v>
       </c>
       <c r="F17" t="n">
-        <v>558.09</v>
+        <v>548.38</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.98</v>
+        <v>0.39</v>
       </c>
       <c r="H17" t="n">
-        <v>0.16</v>
+        <v>-0.71</v>
       </c>
       <c r="I17" t="n">
-        <v>11.02</v>
+        <v>-8.789999999999999</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>6.550068775448152</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0600000000000591</v>
+        <v>-0.0310752019887847</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>55</v>
+        <v>67.81100000000001</v>
       </c>
       <c r="B18" t="n">
-        <v>54939</v>
+        <v>67811</v>
       </c>
       <c r="C18" t="n">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="D18" t="n">
-        <v>17.79</v>
+        <v>19.1</v>
       </c>
       <c r="E18" t="n">
-        <v>954.45</v>
+        <v>960.66</v>
       </c>
       <c r="F18" t="n">
-        <v>558.0700000000001</v>
+        <v>548.36</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.8</v>
+        <v>1.02</v>
       </c>
       <c r="H18" t="n">
-        <v>-1.65</v>
+        <v>0.24</v>
       </c>
       <c r="I18" t="n">
-        <v>4.71</v>
+        <v>-8.390000000000001</v>
       </c>
       <c r="J18" t="n">
-        <v>4.152845064790315</v>
+        <v>5.073946968369117</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.0039999999999963</v>
+        <v>-0.0124300807955137</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>58</v>
+        <v>69.42</v>
       </c>
       <c r="B19" t="n">
-        <v>58157</v>
+        <v>69420</v>
       </c>
       <c r="C19" t="n">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D19" t="n">
-        <v>17.8</v>
+        <v>19.13</v>
       </c>
       <c r="E19" t="n">
-        <v>954.45</v>
+        <v>960.67</v>
       </c>
       <c r="F19" t="n">
-        <v>558.0700000000001</v>
+        <v>548.29</v>
       </c>
       <c r="G19" t="n">
-        <v>0.47</v>
+        <v>0.35</v>
       </c>
       <c r="H19" t="n">
-        <v>0.82</v>
+        <v>0.16</v>
       </c>
       <c r="I19" t="n">
-        <v>10.55</v>
+        <v>-8.32</v>
       </c>
       <c r="J19" t="n">
-        <v>2.936562893136927</v>
+        <v>5.074205960698897</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>-0.0435052827843693</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>60</v>
+        <v>71.029</v>
       </c>
       <c r="B20" t="n">
-        <v>59766</v>
+        <v>71029</v>
       </c>
       <c r="C20" t="n">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D20" t="n">
-        <v>17.81</v>
+        <v>19.16</v>
       </c>
       <c r="E20" t="n">
-        <v>954.45</v>
+        <v>960.67</v>
       </c>
       <c r="F20" t="n">
-        <v>558.02</v>
+        <v>548.29</v>
       </c>
       <c r="G20" t="n">
-        <v>1.57</v>
+        <v>1.14</v>
       </c>
       <c r="H20" t="n">
-        <v>0.43</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>11.3</v>
+        <v>-8.470000000000001</v>
       </c>
       <c r="J20" t="n">
+        <v>5.859518103903431</v>
+      </c>
+      <c r="K20" t="n">
         <v>0</v>
-      </c>
-      <c r="K20" t="n">
-        <v>-0.0250000000000341</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>61</v>
+        <v>72.63800000000001</v>
       </c>
       <c r="B21" t="n">
-        <v>61375</v>
+        <v>72638</v>
       </c>
       <c r="C21" t="n">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D21" t="n">
-        <v>17.82</v>
+        <v>19.19</v>
       </c>
       <c r="E21" t="n">
-        <v>954.45</v>
+        <v>960.6799999999999</v>
       </c>
       <c r="F21" t="n">
-        <v>558.01</v>
+        <v>548.26</v>
       </c>
       <c r="G21" t="n">
-        <v>1.69</v>
+        <v>0.86</v>
       </c>
       <c r="H21" t="n">
-        <v>0.55</v>
+        <v>0.51</v>
       </c>
       <c r="I21" t="n">
-        <v>11.18</v>
+        <v>-8.359999999999999</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>5.859817227895805</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.0099999999999909</v>
+        <v>-0.0186451211932706</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>63</v>
+        <v>74.247</v>
       </c>
       <c r="B22" t="n">
-        <v>62984</v>
+        <v>74247</v>
       </c>
       <c r="C22" t="n">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="D22" t="n">
-        <v>17.82</v>
+        <v>19.21</v>
       </c>
       <c r="E22" t="n">
-        <v>954.46</v>
+        <v>960.6799999999999</v>
       </c>
       <c r="F22" t="n">
-        <v>557.97</v>
+        <v>548.26</v>
       </c>
       <c r="G22" t="n">
-        <v>0.04</v>
+        <v>1.33</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.82</v>
+        <v>9.41</v>
       </c>
       <c r="I22" t="n">
-        <v>10.87</v>
+        <v>-2.94</v>
       </c>
       <c r="J22" t="n">
+        <v>4.143671973431132</v>
+      </c>
+      <c r="K22" t="n">
         <v>0</v>
-      </c>
-      <c r="K22" t="n">
-        <v>-0.0199999999999818</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>66</v>
+        <v>75.85599999999999</v>
       </c>
       <c r="B23" t="n">
-        <v>66202</v>
+        <v>75856</v>
       </c>
       <c r="C23" t="n">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D23" t="n">
-        <v>17.84</v>
+        <v>19.25</v>
       </c>
       <c r="E23" t="n">
-        <v>954.46</v>
+        <v>960.67</v>
       </c>
       <c r="F23" t="n">
-        <v>557.99</v>
+        <v>548.28</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.51</v>
+        <v>-4.47</v>
       </c>
       <c r="H23" t="n">
-        <v>2.59</v>
+        <v>8.630000000000001</v>
       </c>
       <c r="I23" t="n">
-        <v>11.41</v>
+        <v>-1.02</v>
       </c>
       <c r="J23" t="n">
-        <v>2.936779365430287</v>
+        <v>4.144004640553862</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0066666666666606</v>
+        <v>0.0124300807955139</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>68</v>
+        <v>77.46599999999999</v>
       </c>
       <c r="B24" t="n">
-        <v>67811</v>
+        <v>77466</v>
       </c>
       <c r="C24" t="n">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="D24" t="n">
-        <v>17.85</v>
+        <v>19.27</v>
       </c>
       <c r="E24" t="n">
-        <v>954.46</v>
+        <v>960.67</v>
       </c>
       <c r="F24" t="n">
-        <v>557.97</v>
+        <v>548.29</v>
       </c>
       <c r="G24" t="n">
-        <v>0.75</v>
+        <v>-6.67</v>
       </c>
       <c r="H24" t="n">
-        <v>1.57</v>
+        <v>3.57</v>
       </c>
       <c r="I24" t="n">
-        <v>11.49</v>
+        <v>-4.08</v>
       </c>
       <c r="J24" t="n">
-        <v>0</v>
+        <v>4.144160150268372</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.0099999999999909</v>
+        <v>0.0062111801242179</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>69</v>
+        <v>79.075</v>
       </c>
       <c r="B25" t="n">
-        <v>69420</v>
+        <v>79075</v>
       </c>
       <c r="C25" t="n">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D25" t="n">
-        <v>17.86</v>
+        <v>19.29</v>
       </c>
       <c r="E25" t="n">
-        <v>954.46</v>
+        <v>960.67</v>
       </c>
       <c r="F25" t="n">
-        <v>557.95</v>
+        <v>548.3</v>
       </c>
       <c r="G25" t="n">
-        <v>1.29</v>
+        <v>-3.49</v>
       </c>
       <c r="H25" t="n">
-        <v>1.06</v>
+        <v>-2.82</v>
       </c>
       <c r="I25" t="n">
-        <v>10.67</v>
+        <v>10.04</v>
       </c>
       <c r="J25" t="n">
-        <v>2.936895377495464</v>
+        <v>4.144315671243795</v>
       </c>
       <c r="K25" t="n">
-        <v>-0.0199999999999818</v>
+        <v>0.0062150403977568</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>71</v>
+        <v>80.684</v>
       </c>
       <c r="B26" t="n">
-        <v>71029</v>
+        <v>80684</v>
       </c>
       <c r="C26" t="n">
         <v>549</v>
       </c>
       <c r="D26" t="n">
-        <v>17.86</v>
+        <v>19.31</v>
       </c>
       <c r="E26" t="n">
-        <v>954.46</v>
+        <v>960.67</v>
       </c>
       <c r="F26" t="n">
-        <v>557.9400000000001</v>
+        <v>548.34</v>
       </c>
       <c r="G26" t="n">
-        <v>1.06</v>
+        <v>-3.06</v>
       </c>
       <c r="H26" t="n">
-        <v>0.59</v>
+        <v>-3.73</v>
       </c>
       <c r="I26" t="n">
-        <v>11.34</v>
+        <v>10.12</v>
       </c>
       <c r="J26" t="n">
-        <v>2.936895377495464</v>
+        <v>2.93058369242471</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.0049999999999954</v>
+        <v>0.0248601615910984</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>73</v>
+        <v>82.29300000000001</v>
       </c>
       <c r="B27" t="n">
-        <v>72638</v>
+        <v>82293</v>
       </c>
       <c r="C27" t="n">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D27" t="n">
-        <v>17.88</v>
+        <v>19.33</v>
       </c>
       <c r="E27" t="n">
-        <v>954.45</v>
+        <v>960.67</v>
       </c>
       <c r="F27" t="n">
-        <v>558.05</v>
+        <v>548.3200000000001</v>
       </c>
       <c r="G27" t="n">
-        <v>1.18</v>
+        <v>-1.29</v>
       </c>
       <c r="H27" t="n">
-        <v>0.98</v>
+        <v>-2.47</v>
       </c>
       <c r="I27" t="n">
-        <v>-1.41</v>
+        <v>10.71</v>
       </c>
       <c r="J27" t="n">
-        <v>5.874053831347071</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>0.0549999999999499</v>
+        <v>-0.0124300807955137</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>74</v>
+        <v>83.902</v>
       </c>
       <c r="B28" t="n">
-        <v>74247</v>
+        <v>83902</v>
       </c>
       <c r="C28" t="n">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D28" t="n">
-        <v>17.89</v>
+        <v>19.34</v>
       </c>
       <c r="E28" t="n">
-        <v>954.4400000000001</v>
+        <v>960.66</v>
       </c>
       <c r="F28" t="n">
-        <v>558.11</v>
+        <v>548.39</v>
       </c>
       <c r="G28" t="n">
-        <v>1.1</v>
+        <v>-4.16</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.55</v>
+        <v>-0.78</v>
       </c>
       <c r="I28" t="n">
-        <v>11.61</v>
+        <v>10.75</v>
       </c>
       <c r="J28" t="n">
-        <v>2.93710044703777</v>
+        <v>2.930764009984982</v>
       </c>
       <c r="K28" t="n">
-        <v>0.0600000000000591</v>
+        <v>0.0435052827842986</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>76</v>
+        <v>85.511</v>
       </c>
       <c r="B29" t="n">
-        <v>75856</v>
+        <v>85511</v>
       </c>
       <c r="C29" t="n">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="D29" t="n">
-        <v>17.9</v>
+        <v>19.36</v>
       </c>
       <c r="E29" t="n">
-        <v>954.4400000000001</v>
+        <v>960.66</v>
       </c>
       <c r="F29" t="n">
-        <v>558.12</v>
+        <v>548.36</v>
       </c>
       <c r="G29" t="n">
-        <v>2.04</v>
+        <v>-1.37</v>
       </c>
       <c r="H29" t="n">
-        <v>1.18</v>
+        <v>0.47</v>
       </c>
       <c r="I29" t="n">
-        <v>11.26</v>
+        <v>-8.24</v>
       </c>
       <c r="J29" t="n">
-        <v>2.9371584701037</v>
+        <v>5.861748017119465</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0049999999999954</v>
+        <v>-0.0186451211932708</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>77</v>
+        <v>87.12</v>
       </c>
       <c r="B30" t="n">
-        <v>77465</v>
+        <v>87120</v>
       </c>
       <c r="C30" t="n">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="D30" t="n">
-        <v>17.91</v>
+        <v>19.38</v>
       </c>
       <c r="E30" t="n">
-        <v>954.4400000000001</v>
+        <v>960.67</v>
       </c>
       <c r="F30" t="n">
-        <v>558.1</v>
+        <v>548.33</v>
       </c>
       <c r="G30" t="n">
-        <v>3.02</v>
+        <v>0.63</v>
       </c>
       <c r="H30" t="n">
-        <v>1.26</v>
+        <v>0.27</v>
       </c>
       <c r="I30" t="n">
-        <v>11.49</v>
+        <v>-8.43</v>
       </c>
       <c r="J30" t="n">
-        <v>4.153851405385875</v>
+        <v>4.145015655424846</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.0199999999999818</v>
+        <v>-0.0186451211932706</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>79</v>
+        <v>88.729</v>
       </c>
       <c r="B31" t="n">
-        <v>79074</v>
+        <v>88729</v>
       </c>
       <c r="C31" t="n">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D31" t="n">
-        <v>17.92</v>
+        <v>19.39</v>
       </c>
       <c r="E31" t="n">
-        <v>954.45</v>
+        <v>960.67</v>
       </c>
       <c r="F31" t="n">
-        <v>558.04</v>
+        <v>548.3099999999999</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.31</v>
+        <v>-0.27</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.24</v>
+        <v>0.82</v>
       </c>
       <c r="I31" t="n">
-        <v>10.79</v>
+        <v>-7.81</v>
       </c>
       <c r="J31" t="n">
-        <v>2.937259013636284</v>
+        <v>5.076681938945102</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.0300000000000295</v>
+        <v>-0.0124300807955845</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>81</v>
+        <v>90.33799999999999</v>
       </c>
       <c r="B32" t="n">
-        <v>80683</v>
+        <v>90338</v>
       </c>
       <c r="C32" t="n">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D32" t="n">
-        <v>17.93</v>
+        <v>19.41</v>
       </c>
       <c r="E32" t="n">
-        <v>954.45</v>
+        <v>960.67</v>
       </c>
       <c r="F32" t="n">
-        <v>558.03</v>
+        <v>548.28</v>
       </c>
       <c r="G32" t="n">
-        <v>1.65</v>
+        <v>1.26</v>
       </c>
       <c r="H32" t="n">
-        <v>1.92</v>
+        <v>0.43</v>
       </c>
       <c r="I32" t="n">
-        <v>12.98</v>
+        <v>-8.51</v>
       </c>
       <c r="J32" t="n">
-        <v>2.937317047182534</v>
+        <v>5.076872495632891</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.0049999999999954</v>
+        <v>-0.0186451211932708</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>82</v>
+        <v>91.947</v>
       </c>
       <c r="B33" t="n">
-        <v>82293</v>
+        <v>91947</v>
       </c>
       <c r="C33" t="n">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D33" t="n">
-        <v>17.94</v>
+        <v>19.42</v>
       </c>
       <c r="E33" t="n">
-        <v>954.4400000000001</v>
+        <v>960.6799999999999</v>
       </c>
       <c r="F33" t="n">
-        <v>558.09</v>
+        <v>548.26</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.9</v>
+        <v>0.63</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.71</v>
+        <v>0.35</v>
       </c>
       <c r="I33" t="n">
-        <v>11.3</v>
+        <v>-8.43</v>
       </c>
       <c r="J33" t="n">
-        <v>2.937390598590347</v>
+        <v>5.076941212675098</v>
       </c>
       <c r="K33" t="n">
-        <v>0.0600000000000591</v>
+        <v>-0.0124300807955137</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>84</v>
+        <v>93.556</v>
       </c>
       <c r="B34" t="n">
-        <v>83902</v>
+        <v>93556</v>
       </c>
       <c r="C34" t="n">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D34" t="n">
-        <v>17.95</v>
+        <v>19.43</v>
       </c>
       <c r="E34" t="n">
-        <v>954.4400000000001</v>
+        <v>960.6799999999999</v>
       </c>
       <c r="F34" t="n">
-        <v>558.1</v>
+        <v>548.24</v>
       </c>
       <c r="G34" t="n">
-        <v>-2.86</v>
+        <v>0.82</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.59</v>
+        <v>0.16</v>
       </c>
       <c r="I34" t="n">
-        <v>10.24</v>
+        <v>-8.470000000000001</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>5.86245677892799</v>
       </c>
       <c r="K34" t="n">
-        <v>0.0049999999999954</v>
+        <v>-0.0124300807955139</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>86</v>
+        <v>95.16500000000001</v>
       </c>
       <c r="B35" t="n">
-        <v>85511</v>
+        <v>95165</v>
       </c>
       <c r="C35" t="n">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D35" t="n">
-        <v>17.96</v>
+        <v>19.44</v>
       </c>
       <c r="E35" t="n">
-        <v>954.4400000000001</v>
+        <v>960.6799999999999</v>
       </c>
       <c r="F35" t="n">
-        <v>558.11</v>
+        <v>548.27</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.67</v>
+        <v>0.71</v>
       </c>
       <c r="H35" t="n">
-        <v>-1.14</v>
+        <v>0.27</v>
       </c>
       <c r="I35" t="n">
-        <v>11.38</v>
+        <v>-8.43</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>5.862566810287773</v>
       </c>
       <c r="K35" t="n">
-        <v>0.0049999999999954</v>
+        <v>0.0186451211932706</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>87</v>
+        <v>0.232</v>
       </c>
       <c r="B36" t="n">
-        <v>87120</v>
+        <v>232</v>
       </c>
       <c r="C36" t="n">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D36" t="n">
-        <v>17.97</v>
+        <v>19.53</v>
       </c>
       <c r="E36" t="n">
-        <v>954.4400000000001</v>
+        <v>960.66</v>
       </c>
       <c r="F36" t="n">
-        <v>558.14</v>
+        <v>548.4299999999999</v>
       </c>
       <c r="G36" t="n">
-        <v>2.08</v>
+        <v>0.67</v>
       </c>
       <c r="H36" t="n">
-        <v>0.59</v>
+        <v>0.39</v>
       </c>
       <c r="I36" t="n">
-        <v>11.77</v>
+        <v>-8.43</v>
       </c>
       <c r="J36" t="n">
-        <v>2.93756473305386</v>
+        <v>5.078042702447281</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0299999999999727</v>
+        <v>-0.0016853991762608</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>89</v>
+        <v>1.841</v>
       </c>
       <c r="B37" t="n">
-        <v>88729</v>
+        <v>1841</v>
       </c>
       <c r="C37" t="n">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="D37" t="n">
-        <v>17.99</v>
+        <v>19.54</v>
       </c>
       <c r="E37" t="n">
-        <v>954.4400000000001</v>
+        <v>960.67</v>
       </c>
       <c r="F37" t="n">
-        <v>558.14</v>
+        <v>548.33</v>
       </c>
       <c r="G37" t="n">
-        <v>1.96</v>
+        <v>0.86</v>
       </c>
       <c r="H37" t="n">
-        <v>0.78</v>
+        <v>0.27</v>
       </c>
       <c r="I37" t="n">
-        <v>9.960000000000001</v>
+        <v>-8.43</v>
       </c>
       <c r="J37" t="n">
-        <v>4.154508087086087</v>
+        <v>5.863698030570342</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>-0.0621504039775693</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>90</v>
+        <v>3.45</v>
       </c>
       <c r="B38" t="n">
-        <v>90338</v>
+        <v>3450</v>
       </c>
       <c r="C38" t="n">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="D38" t="n">
-        <v>18</v>
+        <v>19.54</v>
       </c>
       <c r="E38" t="n">
-        <v>954.4400000000001</v>
+        <v>960.67</v>
       </c>
       <c r="F38" t="n">
-        <v>558.14</v>
+        <v>548.3200000000001</v>
       </c>
       <c r="G38" t="n">
-        <v>0.47</v>
+        <v>0.82</v>
       </c>
       <c r="H38" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="I38" t="n">
-        <v>11.06</v>
+        <v>-8.470000000000001</v>
       </c>
       <c r="J38" t="n">
-        <v>2.937738900242392</v>
+        <v>5.863698030570342</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>-0.0062150403977569</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>92</v>
+        <v>5.059</v>
       </c>
       <c r="B39" t="n">
-        <v>91947</v>
+        <v>5059</v>
       </c>
       <c r="C39" t="n">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="D39" t="n">
-        <v>18.01</v>
+        <v>19.54</v>
       </c>
       <c r="E39" t="n">
-        <v>954.4299999999999</v>
+        <v>960.67</v>
       </c>
       <c r="F39" t="n">
-        <v>558.1799999999999</v>
+        <v>548.3099999999999</v>
       </c>
       <c r="G39" t="n">
-        <v>-7.49</v>
+        <v>0.59</v>
       </c>
       <c r="H39" t="n">
-        <v>5.88</v>
+        <v>0.24</v>
       </c>
       <c r="I39" t="n">
-        <v>1.33</v>
+        <v>-8.51</v>
       </c>
       <c r="J39" t="n">
-        <v>4.154694253552516</v>
+        <v>6.555813697943462</v>
       </c>
       <c r="K39" t="n">
-        <v>0.0199999999999818</v>
+        <v>-0.0062150403978275</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>94</v>
+        <v>6.668</v>
       </c>
       <c r="B40" t="n">
-        <v>93556</v>
+        <v>6668</v>
       </c>
       <c r="C40" t="n">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="D40" t="n">
-        <v>18.02</v>
+        <v>19.54</v>
       </c>
       <c r="E40" t="n">
-        <v>954.4299999999999</v>
+        <v>960.67</v>
       </c>
       <c r="F40" t="n">
-        <v>558.1900000000001</v>
+        <v>548.34</v>
       </c>
       <c r="G40" t="n">
-        <v>-6.79</v>
+        <v>0.82</v>
       </c>
       <c r="H40" t="n">
-        <v>8.039999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="I40" t="n">
-        <v>3.06</v>
+        <v>-8.32</v>
       </c>
       <c r="J40" t="n">
-        <v>4.154776372755112</v>
+        <v>5.863698030570342</v>
       </c>
       <c r="K40" t="n">
-        <v>0.0050000000000522</v>
+        <v>0.0186451211933414</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>95</v>
+        <v>8.276999999999999</v>
       </c>
       <c r="B41" t="n">
-        <v>95165</v>
+        <v>8277</v>
       </c>
       <c r="C41" t="n">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="D41" t="n">
-        <v>18.04</v>
+        <v>19.55</v>
       </c>
       <c r="E41" t="n">
-        <v>954.4299999999999</v>
+        <v>960.67</v>
       </c>
       <c r="F41" t="n">
-        <v>558.17</v>
+        <v>548.33</v>
       </c>
       <c r="G41" t="n">
-        <v>-5.77</v>
+        <v>0.82</v>
       </c>
       <c r="H41" t="n">
-        <v>7.61</v>
+        <v>0.47</v>
       </c>
       <c r="I41" t="n">
-        <v>4.24</v>
+        <v>-8.390000000000001</v>
       </c>
       <c r="J41" t="n">
-        <v>4.154940626639556</v>
+        <v>5.863808107104608</v>
       </c>
       <c r="K41" t="n">
-        <v>-0.0200000000000954</v>
+        <v>-0.0062150403977569</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>97</v>
+        <v>9.885999999999999</v>
       </c>
       <c r="B42" t="n">
-        <v>96774</v>
+        <v>9886</v>
       </c>
       <c r="C42" t="n">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="D42" t="n">
-        <v>18.05</v>
+        <v>19.55</v>
       </c>
       <c r="E42" t="n">
-        <v>954.4299999999999</v>
+        <v>960.66</v>
       </c>
       <c r="F42" t="n">
-        <v>558.1799999999999</v>
+        <v>548.39</v>
       </c>
       <c r="G42" t="n">
-        <v>-5.14</v>
+        <v>1.26</v>
       </c>
       <c r="H42" t="n">
-        <v>5.53</v>
+        <v>0.78</v>
       </c>
       <c r="I42" t="n">
-        <v>8.199999999999999</v>
+        <v>-8.51</v>
       </c>
       <c r="J42" t="n">
-        <v>2.938044770519443</v>
+        <v>5.863838792797019</v>
       </c>
       <c r="K42" t="n">
-        <v>0.0049999999999954</v>
+        <v>0.0372902423865416</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>98</v>
+        <v>11.495</v>
       </c>
       <c r="B43" t="n">
-        <v>98383</v>
+        <v>11495</v>
       </c>
       <c r="C43" t="n">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="D43" t="n">
-        <v>18.06</v>
+        <v>19.55</v>
       </c>
       <c r="E43" t="n">
-        <v>954.4299999999999</v>
+        <v>960.66</v>
       </c>
       <c r="F43" t="n">
-        <v>558.23</v>
+        <v>548.41</v>
       </c>
       <c r="G43" t="n">
-        <v>-6.08</v>
+        <v>0.9</v>
       </c>
       <c r="H43" t="n">
-        <v>7.57</v>
+        <v>0.31</v>
       </c>
       <c r="I43" t="n">
-        <v>3.96</v>
+        <v>-8.390000000000001</v>
       </c>
       <c r="J43" t="n">
-        <v>2.938102852169235</v>
+        <v>5.863838792797019</v>
       </c>
       <c r="K43" t="n">
-        <v>0.0500000000000682</v>
+        <v>0.0124300807955138</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>100</v>
+        <v>13.104</v>
       </c>
       <c r="B44" t="n">
-        <v>99992</v>
+        <v>13104</v>
       </c>
       <c r="C44" t="n">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="D44" t="n">
-        <v>18.07</v>
+        <v>19.56</v>
       </c>
       <c r="E44" t="n">
-        <v>954.4299999999999</v>
+        <v>960.66</v>
       </c>
       <c r="F44" t="n">
-        <v>558.1900000000001</v>
+        <v>548.4299999999999</v>
       </c>
       <c r="G44" t="n">
-        <v>-4.9</v>
+        <v>0.12</v>
       </c>
       <c r="H44" t="n">
-        <v>6.59</v>
+        <v>0.47</v>
       </c>
       <c r="I44" t="n">
-        <v>6.43</v>
+        <v>-8.470000000000001</v>
       </c>
       <c r="J44" t="n">
-        <v>4.155187046213412</v>
+        <v>5.863948874073636</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.0199999999999818</v>
+        <v>0.0124300807955138</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>102</v>
+        <v>14.713</v>
       </c>
       <c r="B45" t="n">
-        <v>101601</v>
+        <v>14713</v>
       </c>
       <c r="C45" t="n">
         <v>552</v>
       </c>
       <c r="D45" t="n">
-        <v>18.08</v>
+        <v>19.56</v>
       </c>
       <c r="E45" t="n">
-        <v>954.4299999999999</v>
+        <v>960.66</v>
       </c>
       <c r="F45" t="n">
-        <v>558.1799999999999</v>
+        <v>548.41</v>
       </c>
       <c r="G45" t="n">
-        <v>-6.08</v>
+        <v>2.71</v>
       </c>
       <c r="H45" t="n">
-        <v>7.61</v>
+        <v>3.53</v>
       </c>
       <c r="I45" t="n">
-        <v>6.71</v>
+        <v>-7.45</v>
       </c>
       <c r="J45" t="n">
-        <v>4.155269196417041</v>
+        <v>4.146438013388688</v>
       </c>
       <c r="K45" t="n">
-        <v>-0.0050000000000522</v>
+        <v>-0.0124300807955138</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>103</v>
+        <v>16.322</v>
       </c>
       <c r="B46" t="n">
-        <v>103210</v>
+        <v>16322</v>
       </c>
       <c r="C46" t="n">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="D46" t="n">
-        <v>18.1</v>
+        <v>19.57</v>
       </c>
       <c r="E46" t="n">
-        <v>954.4299999999999</v>
+        <v>960.66</v>
       </c>
       <c r="F46" t="n">
-        <v>558.17</v>
+        <v>548.4</v>
       </c>
       <c r="G46" t="n">
-        <v>-5.3</v>
+        <v>-2.08</v>
       </c>
       <c r="H46" t="n">
-        <v>5.41</v>
+        <v>1.53</v>
       </c>
       <c r="I46" t="n">
-        <v>8.039999999999999</v>
+        <v>-7.37</v>
       </c>
       <c r="J46" t="n">
-        <v>2.938335215361334</v>
+        <v>6.556217228660184</v>
       </c>
       <c r="K46" t="n">
-        <v>-0.0099999999999909</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>105</v>
-      </c>
-      <c r="B47" t="n">
-        <v>104819</v>
-      </c>
-      <c r="C47" t="n">
-        <v>552</v>
-      </c>
-      <c r="D47" t="n">
-        <v>18.11</v>
-      </c>
-      <c r="E47" t="n">
-        <v>954.4299999999999</v>
-      </c>
-      <c r="F47" t="n">
-        <v>558.1799999999999</v>
-      </c>
-      <c r="G47" t="n">
-        <v>-5.33</v>
-      </c>
-      <c r="H47" t="n">
-        <v>5.26</v>
-      </c>
-      <c r="I47" t="n">
-        <v>7.06</v>
-      </c>
-      <c r="J47" t="n">
-        <v>4.155515678110823</v>
-      </c>
-      <c r="K47" t="n">
-        <v>0.0049999999999954</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>106</v>
-      </c>
-      <c r="B48" t="n">
-        <v>106428</v>
-      </c>
-      <c r="C48" t="n">
-        <v>551</v>
-      </c>
-      <c r="D48" t="n">
-        <v>18.13</v>
-      </c>
-      <c r="E48" t="n">
-        <v>954.4299999999999</v>
-      </c>
-      <c r="F48" t="n">
-        <v>558.1900000000001</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H48" t="n">
-        <v>-1.92</v>
-      </c>
-      <c r="I48" t="n">
-        <v>10.4</v>
-      </c>
-      <c r="J48" t="n">
-        <v>2.93850952624288</v>
-      </c>
-      <c r="K48" t="n">
-        <v>0.0100000000001045</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>108</v>
-      </c>
-      <c r="B49" t="n">
-        <v>108037</v>
-      </c>
-      <c r="C49" t="n">
-        <v>549</v>
-      </c>
-      <c r="D49" t="n">
-        <v>18.14</v>
-      </c>
-      <c r="E49" t="n">
-        <v>954.4299999999999</v>
-      </c>
-      <c r="F49" t="n">
-        <v>558.17</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="I49" t="n">
-        <v>11.22</v>
-      </c>
-      <c r="J49" t="n">
-        <v>2.938567637213381</v>
-      </c>
-      <c r="K49" t="n">
-        <v>-0.0100000000000477</v>
+        <v>-0.0062150403977569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>